<commit_message>
[PV-261][WIP] File read chooses current active sheet which may not be the one with the data in it.
Two changes to Excel input files.
- Correct PV-Test-03 so has valid sheet name
- Create PV-Test-04 so there is no valid sheet name
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-03.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-03.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968A35A2-732A-E14B-B9C9-922465D37B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BC1ED3-94EE-8041-9830-8690AEB3ABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PV-Test-01" sheetId="1" r:id="rId1"/>
+    <sheet name="PV-Test-03" sheetId="1" r:id="rId1"/>
     <sheet name="Dummy" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -550,7 +550,7 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -794,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABCD83-856B-ED46-BCE9-48AECEB468B0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
[PV-232][WIP] Re-visit Upload latest plan functionality
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-03.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-03.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BC1ED3-94EE-8041-9830-8690AEB3ABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B8304B-170A-404E-AE4A-3BFFEC092497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,9 +249,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +289,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -395,7 +395,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -537,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>

</xml_diff>